<commit_message>
finalize LYK5 tree and code
</commit_message>
<xml_diff>
--- a/Protein_Trees/Info_for_tree.xlsx
+++ b/Protein_Trees/Info_for_tree.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffd16e31ab085cd5/Coaker_Lab/Projects/Analysis_for_other_lab_members_and_side_analyses/ROS_assay_for_Jessica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellestevens/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="835" documentId="8_{0729EF24-4080-9543-BA57-5595E51997E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22351725-C020-B941-B14E-1A97C83CB891}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3092FB91-ADF5-9F4C-8956-3044AFFD194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="520" windowWidth="21780" windowHeight="19440" xr2:uid="{C61B1050-F05F-B440-AA3B-07DA975EC264}"/>
+    <workbookView xWindow="5780" yWindow="520" windowWidth="27820" windowHeight="19440" xr2:uid="{C61B1050-F05F-B440-AA3B-07DA975EC264}"/>
   </bookViews>
   <sheets>
     <sheet name="LYK5_Info" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="CERK1_Info" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="420">
   <si>
     <t>Arabidopsis_thaliana</t>
   </si>
@@ -1482,12 +1483,214 @@
   <si>
     <t>AEO18237.1</t>
   </si>
+  <si>
+    <r>
+      <t>Citrus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sp. (Eremolemon)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Citrus australasica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Australian finger lime)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N/A - Citrus australasica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>F. Muell. (1484)</t>
+    </r>
+  </si>
+  <si>
+    <t>N/A - Citrus sp. (2439)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus xlimon (L.) Osbeck (3013)</t>
+  </si>
+  <si>
+    <r>
+      <t>Citrus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>limon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Frost Lisbon lemon)</t>
+    </r>
+  </si>
+  <si>
+    <t>N/A - Citrus xaurantium L.  (3916)</t>
+  </si>
+  <si>
+    <r>
+      <t>Citrus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>aurantium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Rio Red grapefruit)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Citrus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>aurantium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> (4183)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Citrus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>aurantium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Tango mandarin)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1544,6 +1747,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1565,7 +1781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1580,6 +1796,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1897,8 +2114,8 @@
   <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,10 +2123,10 @@
     <col min="1" max="1" width="20" style="7" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="37.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="3"/>
-    <col min="7" max="7" width="35" style="3" customWidth="1"/>
+    <col min="7" max="7" width="46.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -4912,14 +5129,17 @@
       <c r="C131" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>147</v>
+      <c r="D131" s="8" t="s">
+        <v>410</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -4932,14 +5152,17 @@
       <c r="C132" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>146</v>
+      <c r="D132" s="8" t="s">
+        <v>411</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="G132" s="8" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -4952,14 +5175,17 @@
       <c r="C133" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>148</v>
+      <c r="D133" s="8" t="s">
+        <v>415</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -4972,14 +5198,17 @@
       <c r="C134" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>149</v>
+      <c r="D134" s="8" t="s">
+        <v>417</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -4992,14 +5221,17 @@
       <c r="C135" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>150</v>
+      <c r="D135" s="8" t="s">
+        <v>419</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F135" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -5009,11 +5241,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEFD06D-354F-1544-831F-494B31719561}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB04BD2-9EBD-784E-98E9-22FADE0B4BC4}">
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -6365,11 +6643,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C42596B-A641-3144-BDAC-7C0F1253A054}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed citrus names and added in WN LYK5
</commit_message>
<xml_diff>
--- a/Protein_Trees/Info_for_tree.xlsx
+++ b/Protein_Trees/Info_for_tree.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellestevens/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE292D-C104-364D-B8E5-347627521B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C320C670-1DA3-F54A-A49C-6AEFF91E3A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63260" yWindow="22260" windowWidth="34920" windowHeight="17880" activeTab="1" xr2:uid="{C61B1050-F05F-B440-AA3B-07DA975EC264}"/>
+    <workbookView xWindow="32620" yWindow="18840" windowWidth="43240" windowHeight="17320" xr2:uid="{C61B1050-F05F-B440-AA3B-07DA975EC264}"/>
   </bookViews>
   <sheets>
     <sheet name="LYK5_Info" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="533">
   <si>
     <t>Arabidopsis_thaliana</t>
   </si>
@@ -1162,12 +1162,6 @@
     <t>AEO18237.1</t>
   </si>
   <si>
-    <t>N/A - Citrus sp. (2439)</t>
-  </si>
-  <si>
-    <t>N/A - Citrus xlimon (L.) Osbeck (3013)</t>
-  </si>
-  <si>
     <t>NP_566689.2</t>
   </si>
   <si>
@@ -1534,9 +1528,6 @@
     <t>J. microcarpa x J. regia</t>
   </si>
   <si>
-    <t>XP_002510756.2</t>
-  </si>
-  <si>
     <t>XP_002522569.2</t>
   </si>
   <si>
@@ -1558,12 +1549,6 @@
     <t>Citrus clementina</t>
   </si>
   <si>
-    <t>N/A - Citrus australasica F. Muell. (1484)</t>
-  </si>
-  <si>
-    <t>N/A - Citrus xaurantium L. (3916)</t>
-  </si>
-  <si>
     <t>XP_020396113.1</t>
   </si>
   <si>
@@ -1597,30 +1582,6 @@
     <t>Australian finger lime</t>
   </si>
   <si>
-    <t>Frost Lisbon lemon</t>
-  </si>
-  <si>
-    <t>Rio Red grapefruit</t>
-  </si>
-  <si>
-    <t>Tango mandarin</t>
-  </si>
-  <si>
-    <t>Washington navel</t>
-  </si>
-  <si>
-    <t>Valencia sweet orange</t>
-  </si>
-  <si>
-    <t>N/A - Citrus x aurantium L. (3916)</t>
-  </si>
-  <si>
-    <t>N/A - Citrus x aurantium L. (4183)</t>
-  </si>
-  <si>
-    <t>N/A - Citrus x aurantium L. (1241A)</t>
-  </si>
-  <si>
     <t>XP_040973538.1</t>
   </si>
   <si>
@@ -1631,13 +1592,55 @@
   </si>
   <si>
     <t>XP_016696402.2</t>
+  </si>
+  <si>
+    <t>'Midknight Valencia' orange</t>
+  </si>
+  <si>
+    <t>'Frost Lisbon' lemon</t>
+  </si>
+  <si>
+    <t>'Rio Red' grapefruit</t>
+  </si>
+  <si>
+    <t>'Tango' mandarin</t>
+  </si>
+  <si>
+    <t>'Washington navel' orange</t>
+  </si>
+  <si>
+    <t>N/A - Citrus glauca × C. × limon (2439)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus australasica F. Muell. (Microcitrus australasica) (1484)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus × limon (L.) Osbeck (3013)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus × aurantium L. (3916)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus × aurantium L. (4183)</t>
+  </si>
+  <si>
+    <t>N/A -  Citrus × aurantium L. (1241A)</t>
+  </si>
+  <si>
+    <t>N/A - Citrus × aurantium L. (1241A)</t>
+  </si>
+  <si>
+    <t>XP_002510756.1</t>
+  </si>
+  <si>
+    <t>Nicotiana benthamiana (taxid:4100)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1697,12 +1700,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1724,7 +1721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1737,7 +1734,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2052,16 +2052,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28154993-8776-0346-9F49-895CD533268C}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.1640625" style="1" customWidth="1"/>
@@ -2357,7 +2357,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>66</v>
@@ -2794,7 +2794,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>97</v>
@@ -2817,7 +2817,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>97</v>
@@ -2840,7 +2840,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>97</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>81</v>
@@ -2909,7 +2909,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>97</v>
@@ -2932,7 +2932,7 @@
         <v>22</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>97</v>
@@ -2955,7 +2955,7 @@
         <v>22</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>97</v>
@@ -2978,7 +2978,7 @@
         <v>22</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>97</v>
@@ -3001,7 +3001,7 @@
         <v>22</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>97</v>
@@ -3277,7 +3277,7 @@
         <v>28</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>122</v>
@@ -3369,7 +3369,7 @@
         <v>31</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>70</v>
@@ -3645,7 +3645,7 @@
         <v>39</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>74</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>499</v>
+        <v>531</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>81</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>81</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>81</v>
@@ -4930,10 +4930,10 @@
         <v>163</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>71</v>
@@ -4942,7 +4942,7 @@
         <v>72</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>180</v>
+        <v>532</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -4993,7 +4993,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>81</v>
@@ -5001,8 +5001,8 @@
       <c r="C128" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D128" s="6" t="s">
-        <v>524</v>
+      <c r="D128" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>144</v>
@@ -5016,7 +5016,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>81</v>
@@ -5024,8 +5024,8 @@
       <c r="C129" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D129" s="6" t="s">
-        <v>524</v>
+      <c r="D129" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>144</v>
@@ -5045,10 +5045,10 @@
         <v>81</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>144</v>
@@ -5068,10 +5068,10 @@
         <v>82</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>144</v>
@@ -5103,7 +5103,7 @@
         <v>72</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>375</v>
+        <v>524</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -5117,7 +5117,7 @@
         <v>46</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>144</v>
@@ -5126,7 +5126,7 @@
         <v>72</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>507</v>
+        <v>525</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -5139,7 +5139,7 @@
       <c r="C134" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D134" s="11" t="s">
         <v>520</v>
       </c>
       <c r="E134" s="6" t="s">
@@ -5149,7 +5149,7 @@
         <v>72</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>376</v>
+        <v>526</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -5162,7 +5162,7 @@
       <c r="C135" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D135" s="6" t="s">
+      <c r="D135" s="11" t="s">
         <v>521</v>
       </c>
       <c r="E135" s="6" t="s">
@@ -5172,7 +5172,7 @@
         <v>72</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>508</v>
+        <v>527</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -5185,7 +5185,7 @@
       <c r="C136" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D136" s="6" t="s">
+      <c r="D136" s="11" t="s">
         <v>522</v>
       </c>
       <c r="E136" s="6" t="s">
@@ -5195,7 +5195,30 @@
         <v>72</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>526</v>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G137" s="6" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -5208,8 +5231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEFD06D-354F-1544-831F-494B31719561}">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="C108" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5248,7 +5271,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>147</v>
@@ -5271,10 +5294,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
@@ -5294,10 +5317,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>1</v>
@@ -5317,10 +5340,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -5340,7 +5363,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>148</v>
@@ -5363,7 +5386,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>148</v>
@@ -5386,7 +5409,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>148</v>
@@ -5409,7 +5432,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>148</v>
@@ -5432,10 +5455,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>2</v>
@@ -5455,10 +5478,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>2</v>
@@ -5478,10 +5501,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>3</v>
@@ -5501,10 +5524,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>3</v>
@@ -5524,10 +5547,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>4</v>
@@ -5547,10 +5570,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>5</v>
@@ -5570,7 +5593,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>147</v>
@@ -5593,7 +5616,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>147</v>
@@ -5616,16 +5639,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>66</v>
@@ -5639,10 +5662,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -5662,7 +5685,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>147</v>
@@ -5685,7 +5708,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>121</v>
@@ -5707,11 +5730,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>399</v>
+      <c r="A22" s="6" t="s">
+        <v>397</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>12</v>
@@ -5730,8 +5753,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>400</v>
+      <c r="A23" s="6" t="s">
+        <v>398</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>148</v>
@@ -5753,8 +5776,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>401</v>
+      <c r="A24" s="6" t="s">
+        <v>399</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>148</v>
@@ -5776,8 +5799,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>402</v>
+      <c r="A25" s="6" t="s">
+        <v>400</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>147</v>
@@ -5799,8 +5822,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>403</v>
+      <c r="A26" s="6" t="s">
+        <v>401</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>148</v>
@@ -5822,8 +5845,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>404</v>
+      <c r="A27" s="6" t="s">
+        <v>402</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>121</v>
@@ -5845,8 +5868,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>405</v>
+      <c r="A28" s="6" t="s">
+        <v>403</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>147</v>
@@ -5868,8 +5891,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>406</v>
+      <c r="A29" s="6" t="s">
+        <v>404</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>148</v>
@@ -5891,8 +5914,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>407</v>
+      <c r="A30" s="6" t="s">
+        <v>405</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>148</v>
@@ -5914,11 +5937,11 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>408</v>
+      <c r="A31" s="6" t="s">
+        <v>406</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
@@ -5937,17 +5960,17 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>409</v>
+      <c r="A32" s="6" t="s">
+        <v>407</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>97</v>
@@ -5960,8 +5983,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
-        <v>410</v>
+      <c r="A33" s="6" t="s">
+        <v>408</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>147</v>
@@ -5983,8 +6006,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>509</v>
+      <c r="A34" s="6" t="s">
+        <v>504</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>147</v>
@@ -6006,8 +6029,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>411</v>
+      <c r="A35" s="6" t="s">
+        <v>409</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>147</v>
@@ -6016,7 +6039,7 @@
         <v>22</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>97</v>
@@ -6029,8 +6052,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>412</v>
+      <c r="A36" s="6" t="s">
+        <v>410</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>147</v>
@@ -6039,7 +6062,7 @@
         <v>22</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>97</v>
@@ -6052,8 +6075,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>413</v>
+      <c r="A37" s="6" t="s">
+        <v>411</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>148</v>
@@ -6075,8 +6098,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>414</v>
+      <c r="A38" s="6" t="s">
+        <v>412</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>148</v>
@@ -6098,8 +6121,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>491</v>
+      <c r="A39" s="6" t="s">
+        <v>489</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>148</v>
@@ -6121,11 +6144,11 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>415</v>
+      <c r="A40" s="6" t="s">
+        <v>413</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>25</v>
@@ -6144,11 +6167,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>416</v>
+      <c r="A41" s="6" t="s">
+        <v>414</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>26</v>
@@ -6167,11 +6190,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>417</v>
+      <c r="A42" s="6" t="s">
+        <v>415</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>26</v>
@@ -6190,17 +6213,17 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>418</v>
+      <c r="A43" s="6" t="s">
+        <v>416</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>122</v>
@@ -6213,17 +6236,17 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>419</v>
+      <c r="A44" s="6" t="s">
+        <v>417</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>122</v>
@@ -6236,8 +6259,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>420</v>
+      <c r="A45" s="6" t="s">
+        <v>418</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>147</v>
@@ -6259,8 +6282,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>421</v>
+      <c r="A46" s="6" t="s">
+        <v>419</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>147</v>
@@ -6282,11 +6305,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>424</v>
+      <c r="A47" s="6" t="s">
+        <v>422</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>30</v>
@@ -6305,17 +6328,17 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>422</v>
+      <c r="A48" s="6" t="s">
+        <v>420</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>70</v>
@@ -6328,17 +6351,17 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>423</v>
+      <c r="A49" s="6" t="s">
+        <v>421</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>70</v>
@@ -6351,8 +6374,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
-        <v>425</v>
+      <c r="A50" s="6" t="s">
+        <v>423</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>121</v>
@@ -6374,11 +6397,11 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>426</v>
+      <c r="A51" s="6" t="s">
+        <v>424</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>34</v>
@@ -6397,11 +6420,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
-        <v>427</v>
+      <c r="A52" s="6" t="s">
+        <v>425</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>35</v>
@@ -6420,11 +6443,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>428</v>
+      <c r="A53" s="6" t="s">
+        <v>426</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>35</v>
@@ -6443,17 +6466,17 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="10" t="s">
-        <v>429</v>
+      <c r="A54" s="6" t="s">
+        <v>427</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>74</v>
@@ -6466,11 +6489,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>431</v>
+      <c r="A55" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>40</v>
@@ -6489,11 +6512,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
-        <v>432</v>
+      <c r="A56" s="6" t="s">
+        <v>430</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>40</v>
@@ -6512,11 +6535,11 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>433</v>
+      <c r="A57" s="6" t="s">
+        <v>431</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>40</v>
@@ -6535,11 +6558,11 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
-        <v>434</v>
+      <c r="A58" s="6" t="s">
+        <v>432</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>43</v>
@@ -6558,11 +6581,11 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>437</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>43</v>
@@ -6581,11 +6604,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
-        <v>436</v>
+      <c r="A60" s="6" t="s">
+        <v>434</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>43</v>
@@ -6604,11 +6627,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="10" t="s">
-        <v>438</v>
+      <c r="A61" s="6" t="s">
+        <v>436</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>50</v>
@@ -6627,11 +6650,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="10" t="s">
-        <v>439</v>
+      <c r="A62" s="6" t="s">
+        <v>437</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>50</v>
@@ -6650,11 +6673,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
-        <v>440</v>
+      <c r="A63" s="6" t="s">
+        <v>438</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>51</v>
@@ -6673,11 +6696,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
-        <v>441</v>
+      <c r="A64" s="6" t="s">
+        <v>439</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>44</v>
@@ -6696,11 +6719,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="10" t="s">
-        <v>442</v>
+      <c r="A65" s="6" t="s">
+        <v>440</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>52</v>
@@ -6719,11 +6742,11 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
-        <v>444</v>
+      <c r="A66" s="6" t="s">
+        <v>442</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>53</v>
@@ -6742,11 +6765,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
-        <v>445</v>
+      <c r="A67" s="6" t="s">
+        <v>443</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>53</v>
@@ -6765,11 +6788,11 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>446</v>
+      <c r="A68" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>53</v>
@@ -6788,11 +6811,11 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
-        <v>447</v>
+      <c r="A69" s="6" t="s">
+        <v>445</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>54</v>
@@ -6811,11 +6834,11 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>448</v>
+      <c r="A70" s="6" t="s">
+        <v>446</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>54</v>
@@ -6834,11 +6857,11 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
-        <v>449</v>
+      <c r="A71" s="6" t="s">
+        <v>447</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>55</v>
@@ -6857,11 +6880,11 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
-        <v>450</v>
+      <c r="A72" s="6" t="s">
+        <v>448</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>55</v>
@@ -6880,8 +6903,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
-        <v>510</v>
+      <c r="A73" s="6" t="s">
+        <v>505</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>148</v>
@@ -6903,8 +6926,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>531</v>
+      <c r="A74" s="6" t="s">
+        <v>518</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>147</v>
@@ -6926,8 +6949,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>528</v>
+      <c r="A75" s="6" t="s">
+        <v>515</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>148</v>
@@ -6949,11 +6972,11 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
-        <v>529</v>
+      <c r="A76" s="6" t="s">
+        <v>516</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>59</v>
@@ -6972,8 +6995,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
-        <v>530</v>
+      <c r="A77" s="6" t="s">
+        <v>517</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>148</v>
@@ -6995,11 +7018,11 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
-        <v>451</v>
+      <c r="A78" s="6" t="s">
+        <v>449</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>58</v>
@@ -7018,11 +7041,11 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="10" t="s">
-        <v>452</v>
+      <c r="A79" s="6" t="s">
+        <v>450</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>58</v>
@@ -7041,11 +7064,11 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>453</v>
+      <c r="A80" s="6" t="s">
+        <v>451</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>60</v>
@@ -7064,11 +7087,11 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
-        <v>454</v>
+      <c r="A81" s="6" t="s">
+        <v>452</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>60</v>
@@ -7087,11 +7110,11 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="10" t="s">
-        <v>455</v>
+      <c r="A82" s="6" t="s">
+        <v>453</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>60</v>
@@ -7110,8 +7133,8 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="10" t="s">
-        <v>456</v>
+      <c r="A83" s="6" t="s">
+        <v>454</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>147</v>
@@ -7133,8 +7156,8 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
-        <v>457</v>
+      <c r="A84" s="6" t="s">
+        <v>455</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>147</v>
@@ -7156,11 +7179,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="10" t="s">
-        <v>458</v>
+      <c r="A85" s="6" t="s">
+        <v>456</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>152</v>
@@ -7179,11 +7202,11 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="10" t="s">
-        <v>459</v>
+      <c r="A86" s="6" t="s">
+        <v>457</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>152</v>
@@ -7202,11 +7225,11 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="10" t="s">
-        <v>460</v>
+      <c r="A87" s="6" t="s">
+        <v>458</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>152</v>
@@ -7225,11 +7248,11 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="10" t="s">
-        <v>511</v>
+      <c r="A88" s="6" t="s">
+        <v>506</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>152</v>
@@ -7248,11 +7271,11 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="10" t="s">
-        <v>512</v>
+      <c r="A89" s="6" t="s">
+        <v>507</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>152</v>
@@ -7271,11 +7294,11 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="10" t="s">
-        <v>461</v>
+      <c r="A90" s="6" t="s">
+        <v>459</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>150</v>
@@ -7294,8 +7317,8 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="10" t="s">
-        <v>462</v>
+      <c r="A91" s="6" t="s">
+        <v>460</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>147</v>
@@ -7317,8 +7340,8 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="10" t="s">
-        <v>513</v>
+      <c r="A92" s="6" t="s">
+        <v>508</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>147</v>
@@ -7340,8 +7363,8 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="10" t="s">
-        <v>463</v>
+      <c r="A93" s="6" t="s">
+        <v>461</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>147</v>
@@ -7363,8 +7386,8 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="10" t="s">
-        <v>464</v>
+      <c r="A94" s="6" t="s">
+        <v>462</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>147</v>
@@ -7386,11 +7409,11 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="10" t="s">
-        <v>465</v>
+      <c r="A95" s="6" t="s">
+        <v>463</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>155</v>
@@ -7409,11 +7432,11 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="10" t="s">
-        <v>467</v>
+      <c r="A96" s="6" t="s">
+        <v>465</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>155</v>
@@ -7432,11 +7455,11 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="10" t="s">
-        <v>468</v>
+      <c r="A97" s="6" t="s">
+        <v>466</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>155</v>
@@ -7455,11 +7478,11 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="10" t="s">
-        <v>469</v>
+      <c r="A98" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>156</v>
@@ -7478,11 +7501,11 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="10" t="s">
-        <v>470</v>
+      <c r="A99" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>156</v>
@@ -7501,11 +7524,11 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="10" t="s">
-        <v>471</v>
+      <c r="A100" s="6" t="s">
+        <v>469</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>157</v>
@@ -7524,11 +7547,11 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="10" t="s">
-        <v>472</v>
+      <c r="A101" s="6" t="s">
+        <v>470</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>157</v>
@@ -7547,11 +7570,11 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="10" t="s">
-        <v>473</v>
+      <c r="A102" s="6" t="s">
+        <v>471</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>158</v>
@@ -7570,8 +7593,8 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="10" t="s">
-        <v>474</v>
+      <c r="A103" s="6" t="s">
+        <v>472</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>147</v>
@@ -7593,8 +7616,8 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="10" t="s">
-        <v>475</v>
+      <c r="A104" s="6" t="s">
+        <v>473</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>147</v>
@@ -7616,17 +7639,17 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="6" t="s">
         <v>374</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>163</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>71</v>
@@ -7639,17 +7662,17 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="D106" s="7" t="s">
         <v>477</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>479</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>71</v>
@@ -7662,11 +7685,11 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="10" t="s">
-        <v>480</v>
+      <c r="A107" s="6" t="s">
+        <v>478</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>37</v>
@@ -7685,8 +7708,8 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="10" t="s">
-        <v>481</v>
+      <c r="A108" s="6" t="s">
+        <v>479</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>148</v>
@@ -7708,8 +7731,8 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="10" t="s">
-        <v>482</v>
+      <c r="A109" s="6" t="s">
+        <v>480</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>148</v>
@@ -7731,8 +7754,8 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="10" t="s">
-        <v>483</v>
+      <c r="A110" s="6" t="s">
+        <v>481</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>148</v>
@@ -7754,8 +7777,8 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="10" t="s">
-        <v>484</v>
+      <c r="A111" s="6" t="s">
+        <v>482</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>148</v>
@@ -7777,8 +7800,8 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="10" t="s">
-        <v>485</v>
+      <c r="A112" s="6" t="s">
+        <v>483</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>148</v>
@@ -7801,16 +7824,16 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>524</v>
+        <v>487</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>144</v>
@@ -7823,17 +7846,17 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="10" t="s">
-        <v>515</v>
+      <c r="A114" s="6" t="s">
+        <v>510</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>524</v>
+        <v>487</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>144</v>
@@ -7846,17 +7869,17 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
-        <v>516</v>
+      <c r="A115" s="6" t="s">
+        <v>511</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>147</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>524</v>
+        <v>487</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>144</v>
@@ -7869,17 +7892,17 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="10" t="s">
-        <v>486</v>
+      <c r="A116" s="6" t="s">
+        <v>484</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>144</v>
@@ -7892,17 +7915,17 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="10" t="s">
-        <v>487</v>
+      <c r="A117" s="6" t="s">
+        <v>485</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>147</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>144</v>
@@ -7915,17 +7938,17 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="10" t="s">
-        <v>488</v>
+      <c r="A118" s="6" t="s">
+        <v>486</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>144</v>
@@ -7938,7 +7961,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="10" t="s">
+      <c r="A119" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B119" s="6" t="s">
@@ -7947,7 +7970,7 @@
       <c r="C119" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D119" s="6" t="s">
+      <c r="D119" s="11" t="s">
         <v>521</v>
       </c>
       <c r="E119" s="6" t="s">
@@ -7957,11 +7980,11 @@
         <v>72</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="10" t="s">
+      <c r="A120" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B120" s="6" t="s">
@@ -7970,7 +7993,7 @@
       <c r="C120" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D120" s="6" t="s">
+      <c r="D120" s="11" t="s">
         <v>522</v>
       </c>
       <c r="E120" s="6" t="s">
@@ -7980,20 +8003,20 @@
         <v>72</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>147</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="D121" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="D121" s="11" t="s">
         <v>523</v>
       </c>
       <c r="E121" s="6" t="s">
@@ -8003,7 +8026,7 @@
         <v>72</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>